<commit_message>
results file updated with details for epsilon = 0.1 and exact algo
</commit_message>
<xml_diff>
--- a/Densest_Subgraph_Details.xlsx
+++ b/Densest_Subgraph_Details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t xml:space="preserve">Dataset (.csv)</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Density of Densest Component</t>
   </si>
   <si>
+    <t xml:space="preserve">Exact Max. Density</t>
+  </si>
+  <si>
     <t xml:space="preserve">Avg. Run-time (ms)</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">Number of nodes in densest Component</t>
   </si>
   <si>
+    <t xml:space="preserve">Exact Number of Densest Nodes</t>
+  </si>
+  <si>
     <t xml:space="preserve">epsilon = 0.5</t>
   </si>
   <si>
@@ -59,6 +65,21 @@
   </si>
   <si>
     <t xml:space="preserve">ca-HepPh-new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epsilon = 0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facebook_combined(0.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca-GrQc-new(0.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca-HepTh-new(0.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca-HepPh-new(0.1)</t>
   </si>
 </sst>
 </file>
@@ -68,11 +89,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -90,67 +112,14 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,54 +128,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFC2E0AE"/>
+        <fgColor rgb="FF1C3687"/>
+        <bgColor rgb="FF003366"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC2E0AE"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -214,23 +147,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,81 +172,71 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC2E0AE"/>
@@ -340,7 +248,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -356,7 +264,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -371,7 +279,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF1C3687"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -383,10 +291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,10 +304,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="30.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -418,7 +328,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -427,24 +337,32 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>4039</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -456,21 +374,27 @@
       <c r="E3" s="0" t="n">
         <v>54.597</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
+        <v>77.347</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>91989</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="0" t="n">
         <v>665</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>202</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>5242</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -482,21 +406,27 @@
       <c r="E4" s="0" t="n">
         <v>19.4113</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
+        <v>22.391</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>5844</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>124</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>9877</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -508,21 +438,27 @@
       <c r="E5" s="0" t="n">
         <v>15.5</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>11924</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="J5" s="7" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>12008</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -534,19 +470,169 @@
       <c r="E6" s="0" t="n">
         <v>115.239</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
+        <v>119.004</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>140579</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>4039</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>88234</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>21.8455</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>60.8182</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>77.347</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>118216</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>251</v>
+      <c r="B10" s="6" t="n">
+        <v>5242</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>14496</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2.76536</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>22.3913</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>22.3913</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>6607</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>9877</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>25998</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2.63218</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>12610</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="J11" s="7" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>12008</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>118521</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>9.87017</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>119.004</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>119.004</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>159983</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="J12" s="7" t="n">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
symbol mistake corrected (m->μ)
</commit_message>
<xml_diff>
--- a/Densest_Subgraph_Details.xlsx
+++ b/Densest_Subgraph_Details.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Exact Max. Density</t>
   </si>
   <si>
-    <t xml:space="preserve">Avg. Run-time (ms)</t>
+    <t xml:space="preserve">Avg. Run-time (μs)</t>
   </si>
   <si>
     <t xml:space="preserve">Densest Component (.txt)</t>
@@ -294,7 +294,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>